<commit_message>
Additional fixes, running with updated data, adding a script for lung with more extensive analyses not included in the paper (smoking/stage on first line patients)
</commit_message>
<xml_diff>
--- a/Tables/Supplementary_Table_3.xlsx
+++ b/Tables/Supplementary_Table_3.xlsx
@@ -65,7 +65,7 @@
     <t xml:space="preserve">Fitted as continuous</t>
   </si>
   <si>
-    <t xml:space="preserve">0.992-1.03</t>
+    <t xml:space="preserve">0.991-1.03</t>
   </si>
   <si>
     <t xml:space="preserve">CPI Regimen</t>
@@ -645,7 +645,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.318</v>
+        <v>0.362</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>

</xml_diff>